<commit_message>
fix bug import : admin
</commit_message>
<xml_diff>
--- a/public/template-2.xlsx
+++ b/public/template-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Abdan\Semester 4 (ME)\Pemrograman Profesional\P.Profesional\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Abdan\Semester-4\Pemrograman Profesional\P.Profesional\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9616C54-8D5E-4957-87CE-8E59E28FDF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD77D91E-651D-405E-A4D5-90E6014DAEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{69A33D2D-1EC1-4113-A9D4-14094E67E0EF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>username1</t>
   </si>
@@ -85,21 +85,6 @@
   </si>
   <si>
     <t>password5</t>
-  </si>
-  <si>
-    <t>level1</t>
-  </si>
-  <si>
-    <t>level2</t>
-  </si>
-  <si>
-    <t>level3</t>
-  </si>
-  <si>
-    <t>level4</t>
-  </si>
-  <si>
-    <t>level5</t>
   </si>
   <si>
     <t>*note</t>
@@ -173,14 +158,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -497,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAF5DF7-6804-4DFF-8834-71AF8EF8EE3B}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C9"/>
+      <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +495,7 @@
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,11 +508,8 @@
       <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -540,11 +522,8 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -557,11 +536,8 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -574,11 +550,8 @@
       <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -591,44 +564,41 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="2"/>
     </row>
   </sheetData>

</xml_diff>